<commit_message>
Resolved milli to micro error on xlsx
</commit_message>
<xml_diff>
--- a/AVL_TREE process time.xlsx
+++ b/AVL_TREE process time.xlsx
@@ -19,46 +19,46 @@
     <t>Values number</t>
   </si>
   <si>
-    <t>Read file (ms)</t>
+    <t>Read file (µs)</t>
   </si>
   <si>
-    <t>Insert (ms)</t>
+    <t>Insert (µs)</t>
   </si>
   <si>
-    <t>1st search (ms)</t>
+    <t>1st search (µs)</t>
   </si>
   <si>
-    <t>Delete (ms)</t>
+    <t>Delete (µs)</t>
   </si>
   <si>
-    <t>2nd search (ms)</t>
+    <t>2nd search (µs)</t>
+  </si>
+  <si>
+    <t>Total without reading (µs)</t>
   </si>
   <si>
     <t>Total without reading (ms)</t>
   </si>
   <si>
-    <t>Total without reading (s)</t>
+    <t>Total with reading (µs)</t>
   </si>
   <si>
     <t>Total with reading (ms)</t>
   </si>
   <si>
-    <t>Total with reading (s)</t>
+    <t>Insert by value (µs)</t>
   </si>
   <si>
-    <t>Insert by value (ms)</t>
+    <t>1st search by value (µs)</t>
   </si>
   <si>
-    <t>1st search by value (ms)</t>
+    <t>Delete by value (µs)</t>
   </si>
   <si>
-    <t>Delete by value (ms)</t>
+    <t>2nd search by value (µs)</t>
   </si>
   <si>
-    <t>2nd search by value (ms)</t>
-  </si>
-  <si>
-    <t>Total by value (ms)</t>
+    <t>Total by value (µs)</t>
   </si>
 </sst>
 </file>
@@ -308,11 +308,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="130801822"/>
-        <c:axId val="639678336"/>
+        <c:axId val="2051991576"/>
+        <c:axId val="732703369"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="130801822"/>
+        <c:axId val="2051991576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,10 +364,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="639678336"/>
+        <c:crossAx val="732703369"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="639678336"/>
+        <c:axId val="732703369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,7 +444,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130801822"/>
+        <c:crossAx val="2051991576"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -542,11 +542,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1251722491"/>
-        <c:axId val="31536062"/>
+        <c:axId val="1257609425"/>
+        <c:axId val="1062739655"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1251722491"/>
+        <c:axId val="1257609425"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,10 +598,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31536062"/>
+        <c:crossAx val="1062739655"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31536062"/>
+        <c:axId val="1062739655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1251722491"/>
+        <c:crossAx val="1257609425"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -774,11 +774,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1564158038"/>
-        <c:axId val="1693257942"/>
+        <c:axId val="1202484301"/>
+        <c:axId val="566793570"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1564158038"/>
+        <c:axId val="1202484301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,10 +830,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1693257942"/>
+        <c:crossAx val="566793570"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1693257942"/>
+        <c:axId val="566793570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,7 +908,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564158038"/>
+        <c:crossAx val="1202484301"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1212,6 +1212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -29459,6 +29460,9 @@
       <c r="Z1000" s="4"/>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>